<commit_message>
fts, telescope and smec now under excel control
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
   <si>
     <t>Band</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>Number of collecting dishes</t>
-  </si>
-  <si>
     <t>Primary mirror diameter</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
     <t>Acquisiton frequency (n tau)</t>
   </si>
   <si>
-    <t>V error [%]</t>
-  </si>
-  <si>
     <t>knee freq</t>
   </si>
   <si>
@@ -409,6 +403,18 @@
   </si>
   <si>
     <t>Simulator Control</t>
+  </si>
+  <si>
+    <t>V error type</t>
+  </si>
+  <si>
+    <t>Interscan delay [s]</t>
+  </si>
+  <si>
+    <t>Herschel</t>
+  </si>
+  <si>
+    <t>Pointing error type</t>
   </si>
 </sst>
 </file>
@@ -971,17 +977,17 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -994,49 +1000,49 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="e">
         <f>FTSpectrograph!#REF!*0.000001/(Interferometer!$C$15*0.01)/2</f>
         <v>#REF!</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" t="e">
         <f>B5*180/PI()*60*60</f>
         <v>#REF!</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" t="e">
         <f>B6*180/PI()*60*60</f>
         <v>#REF!</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="G6" t="e">
@@ -1044,7 +1050,7 @@
         <v>#REF!</v>
       </c>
       <c r="H6" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="I6" t="e">
@@ -1054,24 +1060,24 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" t="e">
         <f>B7*180/PI()*60*60</f>
         <v>#REF!</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="G7" t="e">
@@ -1079,7 +1085,7 @@
         <v>#REF!</v>
       </c>
       <c r="H7" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="I7" t="e">
@@ -1089,14 +1095,14 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="e">
         <f>B6/B5</f>
         <v>#REF!</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" t="e">
         <f>ROUND(B8,0)</f>
@@ -1105,14 +1111,14 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="e">
         <f>B7/B5</f>
         <v>#REF!</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="e">
         <f>ROUND(B9,0)</f>
@@ -1121,7 +1127,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1130,67 +1136,67 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="15" t="e">
         <f>B14*B15*100</f>
         <v>#REF!</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F12" s="14" t="e">
         <f>1/2/B20</f>
         <v>#REF!</v>
       </c>
       <c r="G12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="15" t="e">
         <f>FTSpectrograph!#REF!*2</f>
         <v>#REF!</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="15" t="e">
         <f>1/B13/100/FTSpectrograph!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B15" s="15" t="e">
         <f>B13/2/B28</f>
         <v>#REF!</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" t="e">
         <f>ROUND(B15,0)</f>
         <v>#REF!</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" t="e">
         <f>F12/B14*0.01</f>
@@ -1203,66 +1209,66 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B16" s="15" t="e">
         <f>2*B12/B14*0.01</f>
         <v>#REF!</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D16" t="e">
         <f>ROUND(B16,0)</f>
         <v>#REF!</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" t="e">
         <f>D15*D8*D9</f>
         <v>#REF!</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" t="e">
         <f>B18*8</f>
         <v>#REF!</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" t="e">
         <f>D18/1024/1024</f>
         <v>#REF!</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H18" t="e">
         <f>F18/1024</f>
         <v>#REF!</v>
       </c>
       <c r="I18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B20" s="14" t="e">
         <f>(FTSpectrograph!#REF!)/ForSkyParams!B15</f>
         <v>#REF!</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="14"/>
       <c r="F20" t="e">
@@ -1278,7 +1284,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B22" s="14" t="e">
         <f>FTSpectrograph!#REF!/ForSkyParams!B20</f>
@@ -1286,12 +1292,12 @@
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B23" s="14" t="e">
         <f>FTSpectrograph!#REF!/ForSkyParams!B20</f>
@@ -1299,12 +1305,12 @@
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B24" s="14" t="e">
         <f>FTSpectrograph!#REF!/ForSkyParams!B20</f>
@@ -1312,24 +1318,24 @@
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B28" s="15" t="e">
         <f>FTSpectrograph!#REF!/FTSpectrograph!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="F28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B29" s="15" t="e">
         <f>B13/B28</f>
@@ -1338,7 +1344,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B33" t="e">
         <f>1/2/B12</f>
@@ -1347,34 +1353,34 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B37">
         <v>1202</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38">
         <v>1.25E-3</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B39">
         <f>B37*B38/2</f>
@@ -1407,12 +1413,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1420,7 +1426,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1428,7 +1434,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1436,7 +1442,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1444,7 +1450,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1464,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1483,7 +1489,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1515,7 +1521,7 @@
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1653,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1666,22 +1672,21 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="10" t="e">
-        <f>ForSkyParams!B14/Detectors!B3/0.000001*100/2/ColdOptics!#REF!</f>
-        <v>#REF!</v>
+        <v>45</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="10">
         <v>4</v>
@@ -1689,10 +1694,18 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="10">
-        <v>10</v>
+        <v>125</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -1709,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1735,43 +1748,43 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1">
-        <v>0.05</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1819,19 +1832,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" t="s">
         <v>118</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
-        <v>120</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -1930,7 +1943,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="13">
         <f>B6*C6</f>
@@ -1995,12 +2008,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1">
         <v>0.3</v>
@@ -2008,7 +2021,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
@@ -2016,7 +2029,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2024,7 +2037,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1">
         <v>0.7</v>
@@ -2032,7 +2045,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1">
         <v>0.05</v>
@@ -2040,7 +2053,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="1">
         <v>0.98</v>
@@ -2048,7 +2061,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="1">
         <v>0.98</v>
@@ -2056,7 +2069,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="1">
         <v>0.48699999999999999</v>
@@ -2064,7 +2077,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1">
         <v>0.48699999999999999</v>
@@ -2072,7 +2085,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="1">
         <v>0.98</v>
@@ -2080,7 +2093,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" s="1">
         <v>0.98</v>
@@ -2088,7 +2101,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="1">
         <v>0.98</v>
@@ -2096,7 +2109,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
@@ -2128,12 +2141,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1">
         <v>2.726</v>
@@ -2141,7 +2154,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1">
         <v>20</v>
@@ -2149,7 +2162,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="8">
         <v>1.2999999999999999E-5</v>
@@ -2157,7 +2170,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
         <v>220</v>
@@ -2165,7 +2178,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="8">
         <v>7.0000000000000005E-8</v>
@@ -2173,7 +2186,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1">
         <v>5800</v>
@@ -2181,7 +2194,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="8">
         <v>5.0000000000000002E-14</v>
@@ -2189,7 +2202,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="1">
         <v>70</v>
@@ -2220,7 +2233,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2230,18 +2243,18 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1">
         <v>0.05</v>
@@ -2249,18 +2262,18 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1">
         <v>0.05</v>
@@ -2268,7 +2281,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -2299,7 +2312,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2310,18 +2323,18 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1">
         <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1">
         <v>0.56999999999999995</v>
@@ -2329,7 +2342,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -2337,7 +2350,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -2345,25 +2358,25 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7">
         <f>1/(B6*B3*0.000001)</f>
         <v>5000</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" s="1">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Fix issue 10"
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="127">
   <si>
     <t>Band</t>
   </si>
@@ -102,6 +102,9 @@
     <t>Units</t>
   </si>
   <si>
+    <t>Number of collecting dishes</t>
+  </si>
+  <si>
     <t>Primary mirror diameter</t>
   </si>
   <si>
@@ -309,6 +312,9 @@
     <t>Acquisiton frequency (n tau)</t>
   </si>
   <si>
+    <t>V error [%]</t>
+  </si>
+  <si>
     <t>knee freq</t>
   </si>
   <si>
@@ -403,18 +409,6 @@
   </si>
   <si>
     <t>Simulator Control</t>
-  </si>
-  <si>
-    <t>V error type</t>
-  </si>
-  <si>
-    <t>Interscan delay [s]</t>
-  </si>
-  <si>
-    <t>Herschel</t>
-  </si>
-  <si>
-    <t>Pointing error type</t>
   </si>
 </sst>
 </file>
@@ -977,17 +971,17 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -1000,49 +994,49 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B5" t="e">
         <f>FTSpectrograph!#REF!*0.000001/(Interferometer!$C$15*0.01)/2</f>
         <v>#REF!</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" t="e">
         <f>B5*180/PI()*60*60</f>
         <v>#REF!</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D6" t="e">
         <f>B6*180/PI()*60*60</f>
         <v>#REF!</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F6" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="G6" t="e">
@@ -1050,7 +1044,7 @@
         <v>#REF!</v>
       </c>
       <c r="H6" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="I6" t="e">
@@ -1060,24 +1054,24 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D7" t="e">
         <f>B7*180/PI()*60*60</f>
         <v>#REF!</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F7" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="G7" t="e">
@@ -1085,7 +1079,7 @@
         <v>#REF!</v>
       </c>
       <c r="H7" t="e">
-        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
+        <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$4*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="I7" t="e">
@@ -1095,14 +1089,14 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B8" t="e">
         <f>B6/B5</f>
         <v>#REF!</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D8" t="e">
         <f>ROUND(B8,0)</f>
@@ -1111,14 +1105,14 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B9" t="e">
         <f>B7/B5</f>
         <v>#REF!</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" t="e">
         <f>ROUND(B9,0)</f>
@@ -1127,7 +1121,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1136,67 +1130,67 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B12" s="15" t="e">
         <f>B14*B15*100</f>
         <v>#REF!</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F12" s="14" t="e">
         <f>1/2/B20</f>
         <v>#REF!</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B13" s="15" t="e">
         <f>FTSpectrograph!#REF!*2</f>
         <v>#REF!</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B14" s="15" t="e">
         <f>1/B13/100/FTSpectrograph!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B15" s="15" t="e">
         <f>B13/2/B28</f>
         <v>#REF!</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D15" t="e">
         <f>ROUND(B15,0)</f>
         <v>#REF!</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F15" t="e">
         <f>F12/B14*0.01</f>
@@ -1209,66 +1203,66 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B16" s="15" t="e">
         <f>2*B12/B14*0.01</f>
         <v>#REF!</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D16" t="e">
         <f>ROUND(B16,0)</f>
         <v>#REF!</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B18" t="e">
         <f>D15*D8*D9</f>
         <v>#REF!</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" t="e">
         <f>B18*8</f>
         <v>#REF!</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F18" t="e">
         <f>D18/1024/1024</f>
         <v>#REF!</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H18" t="e">
         <f>F18/1024</f>
         <v>#REF!</v>
       </c>
       <c r="I18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="14" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B20" s="14" t="e">
         <f>(FTSpectrograph!#REF!)/ForSkyParams!B15</f>
         <v>#REF!</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D20" s="14"/>
       <c r="F20" t="e">
@@ -1284,7 +1278,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B22" s="14" t="e">
         <f>FTSpectrograph!#REF!/ForSkyParams!B20</f>
@@ -1292,12 +1286,12 @@
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B23" s="14" t="e">
         <f>FTSpectrograph!#REF!/ForSkyParams!B20</f>
@@ -1305,12 +1299,12 @@
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B24" s="14" t="e">
         <f>FTSpectrograph!#REF!/ForSkyParams!B20</f>
@@ -1318,24 +1312,24 @@
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="14" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B28" s="15" t="e">
         <f>FTSpectrograph!#REF!/FTSpectrograph!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="F28" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B29" s="15" t="e">
         <f>B13/B28</f>
@@ -1344,7 +1338,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B33" t="e">
         <f>1/2/B12</f>
@@ -1353,34 +1347,34 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="16" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B37">
         <v>1202</v>
       </c>
       <c r="C37" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B38">
         <v>1.25E-3</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B39">
         <f>B37*B38/2</f>
@@ -1413,12 +1407,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1426,7 +1420,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1434,7 +1428,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1442,7 +1436,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1450,7 +1444,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1470,7 +1464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1489,7 +1483,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1521,7 +1515,7 @@
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1659,10 +1653,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1672,21 +1666,22 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="10">
-        <v>1.5</v>
+        <v>46</v>
+      </c>
+      <c r="B2" s="10" t="e">
+        <f>ForSkyParams!B14/Detectors!B3/0.000001*100/2/ColdOptics!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B3" s="10">
         <v>4</v>
@@ -1694,18 +1689,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5">
-        <v>0.1</v>
+        <v>94</v>
+      </c>
+      <c r="B4" s="10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1722,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1748,43 +1735,43 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1">
-        <v>0.05</v>
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" t="s">
-        <v>127</v>
+        <v>36</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1832,19 +1819,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -1943,7 +1930,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" s="13">
         <f>B6*C6</f>
@@ -2008,12 +1995,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1">
         <v>0.3</v>
@@ -2021,7 +2008,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
@@ -2029,7 +2016,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2037,7 +2024,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1">
         <v>0.7</v>
@@ -2045,7 +2032,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1">
         <v>0.05</v>
@@ -2053,7 +2040,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1">
         <v>0.98</v>
@@ -2061,7 +2048,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1">
         <v>0.98</v>
@@ -2069,7 +2056,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1">
         <v>0.48699999999999999</v>
@@ -2077,7 +2064,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B11" s="1">
         <v>0.48699999999999999</v>
@@ -2085,7 +2072,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1">
         <v>0.98</v>
@@ -2093,7 +2080,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1">
         <v>0.98</v>
@@ -2101,7 +2088,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1">
         <v>0.98</v>
@@ -2109,7 +2096,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
@@ -2141,12 +2128,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1">
         <v>2.726</v>
@@ -2154,7 +2141,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1">
         <v>20</v>
@@ -2162,7 +2149,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="8">
         <v>1.2999999999999999E-5</v>
@@ -2170,7 +2157,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1">
         <v>220</v>
@@ -2178,7 +2165,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" s="8">
         <v>7.0000000000000005E-8</v>
@@ -2186,7 +2173,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1">
         <v>5800</v>
@@ -2194,7 +2181,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="8">
         <v>5.0000000000000002E-14</v>
@@ -2202,7 +2189,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1">
         <v>70</v>
@@ -2233,7 +2220,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2243,18 +2230,18 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1">
         <v>0.05</v>
@@ -2262,18 +2249,18 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1">
         <v>0.05</v>
@@ -2281,7 +2268,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -2312,7 +2299,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2323,18 +2310,18 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1">
         <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>0.56999999999999995</v>
@@ -2342,7 +2329,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -2350,7 +2337,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -2358,25 +2345,25 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <f>1/(B6*B3*0.000001)</f>
         <v>5000</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B8" s="1">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
works with fix-issue-18 branch
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="130">
   <si>
     <t>Band</t>
   </si>
@@ -411,10 +411,13 @@
     <t>Interscan delay [s]</t>
   </si>
   <si>
+    <t>Pointing error type</t>
+  </si>
+  <si>
+    <t>Zero</t>
+  </si>
+  <si>
     <t>Herschel</t>
-  </si>
-  <si>
-    <t>Pointing error type</t>
   </si>
 </sst>
 </file>
@@ -1697,7 +1700,7 @@
         <v>125</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1781,10 +1784,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1802,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showRuler="0" topLeftCell="N53" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1927,7 +1930,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="5">
-        <v>208</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9">

</xml_diff>

<commit_message>
spiro excel :w :q
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="131">
   <si>
     <t>Band</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>Herschel</t>
+  </si>
+  <si>
+    <t>Spiro</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1805,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="N53" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1917,9 +1920,6 @@
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
       <c r="C9" s="5">
         <v>80</v>
       </c>
@@ -1944,6 +1944,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>200</v>
+      </c>
+    </row>
     <row r="15" spans="1:9">
       <c r="A15" s="12" t="s">
         <v>66</v>
@@ -1954,7 +1974,7 @@
       </c>
       <c r="C15" s="12">
         <f>SUM(B15:B19)</f>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1972,7 +1992,7 @@
     <row r="18" spans="2:2">
       <c r="B18" s="11">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:2">

</xml_diff>

<commit_message>
default uv pattern 'spiro', zero pointing and fts errors
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="130">
   <si>
     <t>Band</t>
   </si>
@@ -415,9 +415,6 @@
   </si>
   <si>
     <t>Zero</t>
-  </si>
-  <si>
-    <t>Herschel</t>
   </si>
   <si>
     <t>Spiro</t>
@@ -1667,7 +1664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1790,7 +1787,7 @@
         <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1808,7 +1805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1946,7 +1943,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11">
         <v>1</v>

</xml_diff>

<commit_message>
Version of FIInS_Instrument file with correct parameters for uv pattern.
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="783" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="133">
   <si>
     <t>Band</t>
   </si>
@@ -417,7 +417,16 @@
     <t>Zero</t>
   </si>
   <si>
+    <t>Herschel</t>
+  </si>
+  <si>
     <t>Spiro</t>
+  </si>
+  <si>
+    <t>Const L Spiral</t>
+  </si>
+  <si>
+    <t>period [s]</t>
   </si>
 </sst>
 </file>
@@ -1664,7 +1673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1700,7 +1709,7 @@
         <v>125</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1803,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1818,22 +1827,22 @@
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -1861,8 +1870,11 @@
       <c r="I5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1879,7 +1891,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1899,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1913,10 +1925,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="C9" s="5">
         <v>80</v>
       </c>
@@ -1927,10 +1942,13 @@
         <v>5</v>
       </c>
       <c r="I9" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>100</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
@@ -1941,12 +1959,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>80</v>
@@ -1961,7 +1979,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>79.7</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="12" t="s">
         <v>66</v>
       </c>
@@ -1971,10 +2009,10 @@
       </c>
       <c r="C15" s="12">
         <f>SUM(B15:B19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="B16" s="11">
         <f t="shared" ref="B16:B19" si="0">B7*C7</f>
         <v>0</v>
@@ -1989,7 +2027,7 @@
     <row r="18" spans="2:2">
       <c r="B18" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:2">

</xml_diff>

<commit_message>
Current versions of excel files.
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="540" yWindow="260" windowWidth="25520" windowHeight="15560" tabRatio="783" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="135">
   <si>
     <t>Band</t>
   </si>
@@ -417,7 +417,22 @@
     <t>Zero</t>
   </si>
   <si>
+    <t>Herschel</t>
+  </si>
+  <si>
     <t>Spiro</t>
+  </si>
+  <si>
+    <t>Const L Spiral</t>
+  </si>
+  <si>
+    <t>period [s]</t>
+  </si>
+  <si>
+    <t>Beam model type</t>
+  </si>
+  <si>
+    <t>corrected_on_axis_horn</t>
   </si>
 </sst>
 </file>
@@ -1664,7 +1679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1700,7 +1715,7 @@
         <v>125</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1723,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1788,6 +1803,14 @@
       </c>
       <c r="B7" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1803,10 +1826,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1818,22 +1841,22 @@
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -1861,8 +1884,11 @@
       <c r="I5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1879,7 +1905,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1899,7 +1925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1913,10 +1939,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="C9" s="5">
         <v>80</v>
       </c>
@@ -1927,10 +1956,13 @@
         <v>5</v>
       </c>
       <c r="I9" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>100</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
@@ -1941,12 +1973,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>80</v>
@@ -1961,7 +1993,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>79.7</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="12" t="s">
         <v>66</v>
       </c>
@@ -1971,10 +2023,10 @@
       </c>
       <c r="C15" s="12">
         <f>SUM(B15:B19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="B16" s="11">
         <f t="shared" ref="B16:B19" si="0">B7*C7</f>
         <v>0</v>
@@ -1989,7 +2041,7 @@
     <row r="18" spans="2:2">
       <c r="B18" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:2">

</xml_diff>

<commit_message>
Version allowing different beam model for each collector.
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="260" windowWidth="25520" windowHeight="15560" tabRatio="783" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="540" yWindow="260" windowWidth="25520" windowHeight="15560" tabRatio="783" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="137">
   <si>
     <t>Band</t>
   </si>
@@ -429,10 +429,16 @@
     <t>period [s]</t>
   </si>
   <si>
-    <t>Beam model type</t>
-  </si>
-  <si>
     <t>corrected_on_axis_horn</t>
+  </si>
+  <si>
+    <t>Collector 1 beam model type</t>
+  </si>
+  <si>
+    <t>Collector 2 beam model type</t>
+  </si>
+  <si>
+    <t>perfect</t>
   </si>
 </sst>
 </file>
@@ -1738,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1807,10 +1813,18 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
         <v>133</v>
       </c>
-      <c r="B8" t="s">
-        <v>134</v>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1828,7 +1842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FIInS file with different illumination patterns for each collector.
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -1816,7 +1816,7 @@
         <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1824,7 +1824,7 @@
         <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New version that simulates cosmic rays, detector time constant, and has some code for detector noise though that not activated yet.
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="260" windowWidth="25520" windowHeight="15560" tabRatio="783" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="137">
   <si>
     <t>Band</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Number of detector modes</t>
   </si>
   <si>
-    <t>microns</t>
-  </si>
-  <si>
     <t>Hz</t>
   </si>
   <si>
@@ -438,7 +435,10 @@
     <t>Collector 2 beam model type</t>
   </si>
   <si>
-    <t>perfect</t>
+    <t>CosmicRays</t>
+  </si>
+  <si>
+    <t>microsec</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -618,6 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1001,17 +1002,17 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -1024,46 +1025,46 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="e">
         <f>FTSpectrograph!#REF!*0.000001/(Interferometer!$C$15*0.01)/2</f>
         <v>#REF!</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" t="e">
         <f>B5*180/PI()*60*60</f>
         <v>#REF!</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" t="s">
         <v>95</v>
-      </c>
-      <c r="I5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="e">
         <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="e">
         <f>B6*180/PI()*60*60</f>
         <v>#REF!</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" t="e">
         <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
@@ -1084,21 +1085,21 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="e">
         <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
         <v>#REF!</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" t="e">
         <f>B7*180/PI()*60*60</f>
         <v>#REF!</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F7" t="e">
         <f>FTSpectrograph!#REF!*0.000001/Telescope!$B$3*2.44</f>
@@ -1119,14 +1120,14 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" t="e">
         <f>B6/B5</f>
         <v>#REF!</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" t="e">
         <f>ROUND(B8,0)</f>
@@ -1135,14 +1136,14 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="e">
         <f>B7/B5</f>
         <v>#REF!</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" t="e">
         <f>ROUND(B9,0)</f>
@@ -1151,7 +1152,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1160,41 +1161,41 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="15" t="e">
         <f>B14*B15*100</f>
         <v>#REF!</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" s="14" t="e">
         <f>1/2/B20</f>
         <v>#REF!</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="15" t="e">
         <f>FTSpectrograph!#REF!*2</f>
         <v>#REF!</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="15" t="e">
         <f>1/B13/100/FTSpectrograph!#REF!</f>
@@ -1206,21 +1207,21 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="15" t="e">
         <f>B13/2/B28</f>
         <v>#REF!</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" t="e">
         <f>ROUND(B15,0)</f>
         <v>#REF!</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" t="e">
         <f>F12/B14*0.01</f>
@@ -1233,66 +1234,66 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="15" t="e">
         <f>2*B12/B14*0.01</f>
         <v>#REF!</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D16" t="e">
         <f>ROUND(B16,0)</f>
         <v>#REF!</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" t="e">
         <f>D15*D8*D9</f>
         <v>#REF!</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" t="e">
         <f>B18*8</f>
         <v>#REF!</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F18" t="e">
         <f>D18/1024/1024</f>
         <v>#REF!</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18" t="e">
         <f>F18/1024</f>
         <v>#REF!</v>
       </c>
       <c r="I18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="14" t="e">
         <f>(FTSpectrograph!#REF!)/ForSkyParams!B15</f>
         <v>#REF!</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="14"/>
       <c r="F20" t="e">
@@ -1308,7 +1309,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" s="14" t="e">
         <f>FTSpectrograph!#REF!/ForSkyParams!B20</f>
@@ -1316,12 +1317,12 @@
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B23" s="14" t="e">
         <f>FTSpectrograph!#REF!/ForSkyParams!B20</f>
@@ -1329,12 +1330,12 @@
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="14" t="e">
         <f>FTSpectrograph!#REF!/ForSkyParams!B20</f>
@@ -1342,24 +1343,24 @@
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28" s="15" t="e">
         <f>FTSpectrograph!#REF!/FTSpectrograph!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="F28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29" s="15" t="e">
         <f>B13/B28</f>
@@ -1368,7 +1369,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B33" t="e">
         <f>1/2/B12</f>
@@ -1377,34 +1378,34 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B37">
         <v>1202</v>
       </c>
       <c r="C37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38">
         <v>1.25E-3</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39">
         <f>B37*B38/2</f>
@@ -1424,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1437,12 +1438,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1450,7 +1451,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1458,7 +1459,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1466,7 +1467,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1474,9 +1475,17 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="17">
         <v>0</v>
       </c>
     </row>
@@ -1513,7 +1522,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1545,7 +1554,7 @@
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1696,13 +1705,13 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="10">
         <v>1.5</v>
@@ -1710,7 +1719,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="10">
         <v>4</v>
@@ -1718,15 +1727,15 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5">
         <v>0.1</v>
@@ -1747,7 +1756,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1778,18 +1787,18 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="1">
         <v>0.05</v>
@@ -1797,7 +1806,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
@@ -1805,26 +1814,26 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
         <v>127</v>
-      </c>
-      <c r="B7" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1872,19 +1881,19 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
         <v>116</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>117</v>
-      </c>
-      <c r="E5" t="s">
-        <v>118</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -1899,7 +1908,7 @@
         <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1989,7 +1998,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2009,7 +2018,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2029,7 +2038,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="13">
         <f>B6*C6</f>
@@ -2094,12 +2103,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1">
         <v>0.3</v>
@@ -2107,7 +2116,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
@@ -2115,7 +2124,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -2123,7 +2132,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1">
         <v>0.7</v>
@@ -2131,7 +2140,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1">
         <v>0.05</v>
@@ -2139,7 +2148,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1">
         <v>0.98</v>
@@ -2147,7 +2156,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1">
         <v>0.98</v>
@@ -2155,7 +2164,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="1">
         <v>0.48699999999999999</v>
@@ -2163,7 +2172,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="1">
         <v>0.48699999999999999</v>
@@ -2171,7 +2180,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="1">
         <v>0.98</v>
@@ -2179,7 +2188,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="1">
         <v>0.98</v>
@@ -2187,7 +2196,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="1">
         <v>0.98</v>
@@ -2195,7 +2204,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
@@ -2227,12 +2236,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1">
         <v>2.726</v>
@@ -2240,7 +2249,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1">
         <v>20</v>
@@ -2248,7 +2257,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="8">
         <v>1.2999999999999999E-5</v>
@@ -2256,7 +2265,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1">
         <v>220</v>
@@ -2264,7 +2273,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="8">
         <v>7.0000000000000005E-8</v>
@@ -2272,7 +2281,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1">
         <v>5800</v>
@@ -2280,7 +2289,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="8">
         <v>5.0000000000000002E-14</v>
@@ -2288,7 +2297,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1">
         <v>70</v>
@@ -2319,7 +2328,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2329,18 +2338,18 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1">
         <v>0.05</v>
@@ -2348,18 +2357,18 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1">
         <v>0.05</v>
@@ -2367,7 +2376,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -2388,7 +2397,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2411,11 +2420,11 @@
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="8">
         <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2436,7 +2445,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -2444,25 +2453,25 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7">
         <f>1/(B6*B3*0.000001)</f>
         <v>5000</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="1">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added beam model polarization selection.
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="260" windowWidth="25520" windowHeight="15560" tabRatio="783" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="138">
   <si>
     <t>Band</t>
   </si>
@@ -438,7 +438,10 @@
     <t>Collector 2 beam model type</t>
   </si>
   <si>
-    <t>perfect</t>
+    <t>Beam model polarization</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -1744,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1816,7 +1819,7 @@
         <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1825,6 +1828,14 @@
       </c>
       <c r="B9" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change beam pol to Y
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -441,7 +441,7 @@
     <t>Beam model polarization</t>
   </si>
   <si>
-    <t>X</t>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1749,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Just the current test version.
</commit_message>
<xml_diff>
--- a/excel/FIInS_Instrument_cor3.xlsx
+++ b/excel/FIInS_Instrument_cor3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-220" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="783" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ForSkyParams" sheetId="8" r:id="rId1"/>
@@ -1749,7 +1749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1853,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1917,17 +1917,20 @@
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
       <c r="C6" s="1">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
         <v>10</v>
-      </c>
-      <c r="E6" s="1">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1969,7 +1972,7 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="5">
         <v>80</v>
@@ -2044,11 +2047,11 @@
       </c>
       <c r="B15" s="13">
         <f>B6*C6</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C15" s="12">
         <f>SUM(B15:B19)</f>
-        <v>80</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2066,7 +2069,7 @@
     <row r="18" spans="2:2">
       <c r="B18" s="11">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:2">

</xml_diff>